<commit_message>
Mudanças no back log adição da apresentação ao gitHub
</commit_message>
<xml_diff>
--- a/Documentação/Backlog descubra laTam.xlsx
+++ b/Documentação/Backlog descubra laTam.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1732875-FEEE-4023-A8FC-0A6E823B9675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{716F3798-EFB1-4039-A633-912F2E647FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="60">
   <si>
     <t xml:space="preserve">Projeto Individual descubra laTam - Backlog </t>
   </si>
@@ -60,6 +60,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Reponsável</t>
+  </si>
+  <si>
     <t>Sprint</t>
   </si>
   <si>
@@ -69,106 +72,145 @@
     <t>Pontos feitos</t>
   </si>
   <si>
-    <t xml:space="preserve">Projetos atualizado no GitHub </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inserir andamento do projeto no GitHub </t>
+    <t>Backlog</t>
+  </si>
+  <si>
+    <t>Separação dos requisitos do projeto</t>
   </si>
   <si>
     <t>Essencial</t>
   </si>
   <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Documentação</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da documentação com contexto, objetivo e justificativa</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Modelagem das tabelas</t>
+  </si>
+  <si>
+    <t>Desenvolver o modelo de como irá ficar as tabelas do banco</t>
+  </si>
+  <si>
     <t>PP</t>
   </si>
   <si>
-    <t>Pendente</t>
-  </si>
-  <si>
-    <t>Total:</t>
-  </si>
-  <si>
-    <t>Planilha de Riscos do Projeto</t>
-  </si>
-  <si>
-    <t>Avaliar riscos e confeccionar  planilha de riscos</t>
-  </si>
-  <si>
-    <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>Especificação da Dashboard</t>
-  </si>
-  <si>
-    <t>Criar as especificações da dashboard e KPI</t>
-  </si>
-  <si>
-    <t>Site Estático Institucional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criar o site institucional </t>
+    <t>Criação do repositório no github</t>
+  </si>
+  <si>
+    <t>Criar o repositório no GitHub</t>
+  </si>
+  <si>
+    <t>Configuração do trello</t>
+  </si>
+  <si>
+    <t>Colocar os requisitos no trello para facilitar a gestão</t>
+  </si>
+  <si>
+    <t>Script do banco de dados</t>
+  </si>
+  <si>
+    <t>Desenvolver o script das tabelas com base na modelagem</t>
+  </si>
+  <si>
+    <t>Home do site</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da home do site, contendo oque é, ods e sobre mim</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Cadastro e login</t>
+  </si>
+  <si>
+    <t>Criação da pagina de cadastro e login</t>
+  </si>
+  <si>
+    <t>Dashboard estática</t>
+  </si>
+  <si>
+    <t>Desenvolver a dashboard no site com dados pré-alocados</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
-    <t>Site Estático Dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criar dashboard site </t>
-  </si>
-  <si>
-    <t>Site Estático Cadastro e Login  linkadas ao banco de dados</t>
-  </si>
-  <si>
-    <t>Criar tela de login e cadastro logadas ao banco de dados</t>
-  </si>
-  <si>
-    <t>Fluxograma do suporte</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Visualiza os passos do atendimento, do início à solução, facilitando o processo.</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Ferramenta de Help Desk</t>
-  </si>
-  <si>
-    <t>Software para gerenciar e acompanhar chamados de suporte de forma centralizada.</t>
-  </si>
-  <si>
-    <t>Documento de Mudança</t>
-  </si>
-  <si>
-    <t>Registro detalhado de alterações planejadas, justificativa e impacto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tabelas criadas no Banco de Dados</t>
-  </si>
-  <si>
-    <t>Definir tabelas do SQL e cria-las</t>
-  </si>
-  <si>
-    <t>Documentação do Projeto Atualizada</t>
-  </si>
-  <si>
-    <t>Finalizar/últimas adições na documentação do projeto</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PPT da Apresentação do Projeto</t>
-  </si>
-  <si>
-    <t>Organizar a apresentação/slides do projeto</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Dashboard (ChartJS) acessando o banco</t>
-  </si>
-  <si>
-    <t>Integrar a API com o banco de dados e o site</t>
+    <t>Adição da API web-data-viz</t>
+  </si>
+  <si>
+    <t>Colocar a API disponibilizada pela faculdade no projeto</t>
+  </si>
+  <si>
+    <t>Configuração do cadastro e login</t>
+  </si>
+  <si>
+    <t>Desenvolver os scripts para registro e confirmação do cadastro do usuario</t>
+  </si>
+  <si>
+    <t>Dashboard dinamica</t>
+  </si>
+  <si>
+    <t>Desenvolver o sistema de plotagem dos dados na dash</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>Configuração das kpi's</t>
+  </si>
+  <si>
+    <t>Colocar o sistema de kpi's na dashboard</t>
+  </si>
+  <si>
+    <t>Preparação da VM</t>
+  </si>
+  <si>
+    <t>Realizar as configurações para preparar para recepção do site</t>
+  </si>
+  <si>
+    <t>Banco de dados na VM</t>
+  </si>
+  <si>
+    <t>Executar os scripts de criação do banco de dados na VM</t>
+  </si>
+  <si>
+    <t>Gráfico de burndown</t>
+  </si>
+  <si>
+    <t>Adicionar o grafico de burndown do projeto</t>
+  </si>
+  <si>
+    <t>Preparação do PPT</t>
+  </si>
+  <si>
+    <t>Desenvolver a apresentação do projeto</t>
+  </si>
+  <si>
+    <t>Backup do projeto</t>
+  </si>
+  <si>
+    <t>Fazer o backup em um pendrive</t>
+  </si>
+  <si>
+    <t>Importante</t>
   </si>
 </sst>
 </file>
@@ -292,13 +334,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -332,23 +371,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -440,9 +463,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Estimativa Sprint</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="F2CEEF"/>
@@ -514,10 +534,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$K$4:$K$5</c:f>
+              <c:f>Planilha1!$K$3:$K$4</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
+                  <c:v>Total:</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Sprint 3</c:v>
                 </c:pt>
               </c:strCache>
@@ -525,12 +548,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$L$4:$L$5</c:f>
+              <c:f>Planilha1!$L$3:$L$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,9 +570,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Desempenho </c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -615,10 +638,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$K$4:$K$5</c:f>
+              <c:f>Planilha1!$K$3:$K$4</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
+                  <c:v>Total:</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Sprint 3</c:v>
                 </c:pt>
               </c:strCache>
@@ -626,12 +652,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$M$4:$M$5</c:f>
+              <c:f>Planilha1!$M$3:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1404,15 +1433,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1759,10 +1788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1770,6 +1799,7 @@
     <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
@@ -1777,467 +1807,602 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>11</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="3">
-        <v>3</v>
-      </c>
-      <c r="K3" s="9" t="s">
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="11">
-        <f>SUM(F2:F15)</f>
-        <v>104</v>
-      </c>
-      <c r="M3" s="11">
-        <v>0</v>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="10">
+        <f>SUM(F2:F20)</f>
+        <v>35</v>
+      </c>
+      <c r="M3" s="10">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3">
-        <v>3</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="3">
-        <v>3</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="11">
-        <f>SUM(F3:F15)</f>
-        <v>104</v>
-      </c>
-      <c r="M4" s="11">
-        <v>0</v>
+      <c r="K4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="10">
+        <f>SUM(F3:F20)</f>
+        <v>35</v>
+      </c>
+      <c r="M4" s="10">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="3">
-        <v>3</v>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="3">
-        <v>13</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="3">
-        <v>3</v>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="3">
-        <v>13</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="3">
+      <c r="F7" s="2">
         <v>3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="3">
-        <v>13</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="3">
+      <c r="F8" s="2">
         <v>3</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="3">
-        <v>8</v>
-      </c>
-      <c r="G9" s="3">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="3">
-        <v>3</v>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="3">
-        <v>8</v>
-      </c>
-      <c r="G10" s="3">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="3">
-        <v>3</v>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="3">
-        <v>8</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="B11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2">
         <v>2</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="3">
-        <v>3</v>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
+      <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="3">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="3">
+      <c r="F12" s="2">
         <v>3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="3">
-        <v>8</v>
-      </c>
-      <c r="G13" s="3">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="3">
-        <v>3</v>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="4">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>42</v>
+      <c r="A14" s="3">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="3">
-        <v>3</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="3">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="4">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>45</v>
+      <c r="A15" s="3">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="3">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="3">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="3">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2">
+        <v>3</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="3">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="3">
-        <v>13</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="3">
+      <c r="F20" s="2">
         <v>3</v>
+      </c>
+      <c r="G20" s="2">
+        <v>3</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H3:H15">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Pendente">
-      <formula>NOT(ISERROR(SEARCH("Pendente",H3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H15">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",H3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>